<commit_message>
Compiled 47 literature results, need to check if the ones i have already read are in there and if they are not then add them
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C7DB00-7611-4B5A-84BE-8CDA191034E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DCB35B-9B64-484E-BE1C-3D765BAF0181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="260">
   <si>
     <t>Enhancing upper limb mobility through gamified tasks and Azure Kinect: a preliminary study in post-stroke subjects</t>
   </si>
@@ -756,6 +756,66 @@
   </si>
   <si>
     <t>2-s2.0-85130015354</t>
+  </si>
+  <si>
+    <t>Gamified in-home rehabilitation for stroke survivors: analytical review</t>
+  </si>
+  <si>
+    <t>A game changer:'the use of digital technologies in the management of upper limb rehabilitation'</t>
+  </si>
+  <si>
+    <t>Serious gaming technology in upper extremity rehabilitation: scoping review</t>
+  </si>
+  <si>
+    <t>Compliance with Upper Limb Home-Based Exergaming Interventions for Stroke Patients: A Narrative Review</t>
+  </si>
+  <si>
+    <t>Exoskeletons with virtual reality, augmented reality, and gamification for stroke patients' rehabilitation: systematic review</t>
+  </si>
+  <si>
+    <t>Analysis, Design and Implementation of Serious Game for Upper Limb and Cognitive Training Using Leap Motion for Multiple Sclerosis Patients</t>
+  </si>
+  <si>
+    <t>A survey of technologies facilitating home and community-based stroke rehabilitation</t>
+  </si>
+  <si>
+    <t>Metamorphosis: intensive telerehabilitation to maximize upper limb function and integration in adults with chronic stroke</t>
+  </si>
+  <si>
+    <t>Mirror VR: The design of a fully immersive virtual reality game for upper limb rehabilitation post-stroke using mirror therapy</t>
+  </si>
+  <si>
+    <t>Enabling Home Rehabilitation with Smartphone-Powered Upper Limb Training</t>
+  </si>
+  <si>
+    <t>Evaluation of multiplayer games in robot-assisted neurorehabilitation</t>
+  </si>
+  <si>
+    <t>Virtual reality exergames for enhancing engagement in stroke rehabilitation: A narrative review</t>
+  </si>
+  <si>
+    <t>Cyber-physical solution for an engagement enhancing rehabilitation system</t>
+  </si>
+  <si>
+    <t>The Use of Gamification in the self-management of patients with chronic diseases: scoping review</t>
+  </si>
+  <si>
+    <t>Exploring serious games for stroke rehabilitation: a scoping review</t>
+  </si>
+  <si>
+    <t>Robotic Home-Based Rehabilitation Systems Design: From a Literature Review to a Conceptual Framework for Community-Based Remote Therapy During COVID-19 Pandemic</t>
+  </si>
+  <si>
+    <t>Trends in robot-assisted and virtual reality-assisted neuromuscular therapy: a systematic review of health-related multiplayer games</t>
+  </si>
+  <si>
+    <t>Serious games for stroke telerehabilitation of upper limb-a review for future research</t>
+  </si>
+  <si>
+    <t>Perception of game-based rehabilitation in upper limb prosthetic training: Survey of users and researchers</t>
+  </si>
+  <si>
+    <t>Improving the Motivation and Participation of Elderly Patients in Rehabilitation Program Through Social Games</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1192,7 @@
   <dimension ref="A1:T280"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2562,65 +2622,125 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
+      <c r="D28" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
+      <c r="D29" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
+      <c r="D30" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
+      <c r="D31" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Started looking into what literatures are accessible
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DCB35B-9B64-484E-BE1C-3D765BAF0181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8611C0CB-5B4E-4FFC-9A52-4164A1AF2208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Search" sheetId="1" r:id="rId1"/>
+    <sheet name="Records Sought for retrieval" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="264">
   <si>
     <t>Enhancing upper limb mobility through gamified tasks and Azure Kinect: a preliminary study in post-stroke subjects</t>
   </si>
@@ -816,13 +817,25 @@
   </si>
   <si>
     <t>Improving the Motivation and Participation of Elderly Patients in Rehabilitation Program Through Social Games</t>
+  </si>
+  <si>
+    <t>Serious games for upper limb rehabilitation after stroke: a meta-analysis</t>
+  </si>
+  <si>
+    <t>Development of a 3D, networked multi user virtual reality environment for home therapy after stroke</t>
+  </si>
+  <si>
+    <t>Serious Game Design and Clinical Improvement in Physical Rehabilitation: Systematic Review</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,13 +843,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -851,10 +882,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1189,10 +1222,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C08291-9268-4DC3-B18D-4AB90860BD3C}">
-  <dimension ref="A1:T280"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D47" activeCellId="11" sqref="D2 D4 D6 D8 D9:D15 D19 D27:D34 D36:D39 D42 D44 D45 D47:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,7 +1372,7 @@
       <c r="C3" t="s">
         <v>194</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E3">
@@ -1447,7 +1481,7 @@
       <c r="C5" t="s">
         <v>155</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>154</v>
       </c>
       <c r="E5">
@@ -1544,7 +1578,7 @@
       <c r="C7" t="s">
         <v>139</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>138</v>
       </c>
       <c r="E7">
@@ -1971,7 +2005,7 @@
       <c r="G15">
         <v>17</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>44623</v>
       </c>
       <c r="I15" t="s">
@@ -2012,7 +2046,7 @@
       <c r="C16" t="s">
         <v>63</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E16">
@@ -2071,7 +2105,7 @@
       <c r="C17" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E17">
@@ -2121,7 +2155,7 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E18">
@@ -2227,7 +2261,7 @@
       <c r="C20" t="s">
         <v>27</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E20">
@@ -2274,7 +2308,7 @@
       <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E21">
@@ -2330,7 +2364,7 @@
       <c r="C22" t="s">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E22">
@@ -2386,7 +2420,7 @@
       <c r="C23" t="s">
         <v>201</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>202</v>
       </c>
       <c r="E23">
@@ -2436,7 +2470,7 @@
       <c r="C24" t="s">
         <v>209</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E24">
@@ -2489,7 +2523,7 @@
       <c r="C25" t="s">
         <v>218</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>219</v>
       </c>
       <c r="E25">
@@ -2533,7 +2567,7 @@
       <c r="C26" t="s">
         <v>226</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>227</v>
       </c>
       <c r="E26">
@@ -2621,823 +2655,305 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
       <c r="D28" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
       <c r="D29" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
       <c r="D30" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
       <c r="D31" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
       <c r="D32" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="D35" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="D40" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D40" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="D41" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="D43" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D43" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-      <c r="D46" t="s">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D46" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="1"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="1"/>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="1"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="1"/>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="1"/>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="1"/>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="1"/>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="1"/>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="1"/>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="1"/>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="1"/>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="1"/>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="1"/>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="1"/>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="1"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="1"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="1"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="1"/>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="1"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="1"/>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="1"/>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="1"/>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="1"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="1"/>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="1"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="1"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="1"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="1"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" s="1"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" s="1"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="1"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" s="1"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="1"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="1"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="1"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="1"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="1"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" s="1"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="1"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="1"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" s="1"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" s="1"/>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" s="1"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" s="1"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162" s="1"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163" s="1"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164" s="1"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165" s="1"/>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166" s="1"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167" s="1"/>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168" s="1"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169" s="1"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170" s="1"/>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171" s="1"/>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172" s="1"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173" s="1"/>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A174" s="1"/>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A175" s="1"/>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A176" s="1"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" s="1"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178" s="1"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A181" s="1"/>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A182" s="1"/>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A183" s="1"/>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A184" s="1"/>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A185" s="1"/>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A193" s="1"/>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A194" s="1"/>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A195" s="1"/>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A197" s="1"/>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A198" s="1"/>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A199" s="1"/>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A200" s="1"/>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A201" s="1"/>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A202" s="1"/>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A203" s="1"/>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A204" s="1"/>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A205" s="1"/>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A206" s="1"/>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A207" s="1"/>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A208" s="1"/>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A209" s="1"/>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A210" s="1"/>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A211" s="1"/>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A212" s="1"/>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A213" s="1"/>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A214" s="1"/>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A215" s="1"/>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A216" s="1"/>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A217" s="1"/>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A218" s="1"/>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A219" s="1"/>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A220" s="1"/>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A221" s="1"/>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A222" s="1"/>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A223" s="1"/>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A224" s="1"/>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A225" s="1"/>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A226" s="1"/>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A227" s="1"/>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A228" s="1"/>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A229" s="1"/>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A230" s="1"/>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A231" s="1"/>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A232" s="1"/>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A233" s="1"/>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A234" s="1"/>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A235" s="1"/>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A236" s="1"/>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A237" s="1"/>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A238" s="1"/>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A239" s="1"/>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A240" s="1"/>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A241" s="1"/>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A242" s="1"/>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A243" s="1"/>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A244" s="1"/>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A245" s="1"/>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A246" s="1"/>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A247" s="1"/>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A248" s="1"/>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A249" s="1"/>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A250" s="1"/>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A251" s="1"/>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A252" s="1"/>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A253" s="1"/>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A254" s="1"/>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A255" s="1"/>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A256" s="1"/>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A257" s="1"/>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A258" s="1"/>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A259" s="1"/>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A260" s="1"/>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A261" s="1"/>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A262" s="1"/>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A263" s="1"/>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A264" s="1"/>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A265" s="1"/>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A266" s="1"/>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A267" s="1"/>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A268" s="1"/>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A269" s="1"/>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A270" s="1"/>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A271" s="1"/>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A272" s="1"/>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A273" s="1"/>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A274" s="1"/>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A275" s="1"/>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A276" s="1"/>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A277" s="1"/>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A278" s="1"/>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A279" s="1"/>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A280" s="1"/>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>262</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83627A4-1841-48FA-912D-B4DCB777AFD8}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="164" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>262</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Identified papers which i have access to
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8611C0CB-5B4E-4FFC-9A52-4164A1AF2208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE0ABB2-94D4-4B99-87A1-8BF71E957A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Search" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="264">
   <si>
     <t>Enhancing upper limb mobility through gamified tasks and Azure Kinect: a preliminary study in post-stroke subjects</t>
   </si>
@@ -1225,8 +1225,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D47" activeCellId="11" sqref="D2 D4 D6 D8 D9:D15 D19 D27:D34 D36:D39 D42 D44 D45 D47:D50"/>
+    <sheetView topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1425,7 @@
       <c r="C4" t="s">
         <v>163</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>162</v>
       </c>
       <c r="E4">
@@ -1849,7 +1849,7 @@
       <c r="C12" t="s">
         <v>98</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E12">
@@ -1993,7 +1993,7 @@
       <c r="C15" t="s">
         <v>72</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E15">
@@ -2705,7 +2705,7 @@
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2777,10 +2777,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83627A4-1841-48FA-912D-B4DCB777AFD8}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2800,160 +2800,163 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>129</v>
+      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>122</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>114</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>106</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>97</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>88</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>80</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>71</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>235</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>240</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
         <v>262</v>
       </c>
+      <c r="B28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reading list generated and notes document made just now need to read the papers and make notes
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE0ABB2-94D4-4B99-87A1-8BF71E957A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC11DD66-1F67-4947-8737-1942B3E72429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Search" sheetId="1" r:id="rId1"/>
     <sheet name="Records Sought for retrieval" sheetId="2" r:id="rId2"/>
+    <sheet name="Reading list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="271">
   <si>
     <t>Enhancing upper limb mobility through gamified tasks and Azure Kinect: a preliminary study in post-stroke subjects</t>
   </si>
@@ -829,13 +830,46 @@
   </si>
   <si>
     <t>Success</t>
+  </si>
+  <si>
+    <t>excluded</t>
+  </si>
+  <si>
+    <t>Implementing Home-Based Clinical Research for Caregivers and Persons with Stroke Lessons Learned</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Virtual reality games for rehabilitation of upper extremities in stroke patients. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.5"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of bodywork and movement therapies</t>
+    </r>
+  </si>
+  <si>
+    <t>Personalised physiotherapy rehabilitation using artificial intelligence and virtual reality gaming</t>
+  </si>
+  <si>
+    <t>A Review on Serious Games for Exercise Rehabilitation</t>
+  </si>
+  <si>
+    <t>Evaluating the impact of player experience in the design of a serious game for upper extremity stroke rehabilitation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +882,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.5"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -882,12 +929,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1225,7 +1274,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -2777,10 +2826,227 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83627A4-1841-48FA-912D-B4DCB777AFD8}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" activeCellId="7" sqref="A2 A3 A7:A12 A14:A17 A19:A21 A23:A24 A25:A27 A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="175.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>241</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>244</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>245</v>
+      </c>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>251</v>
+      </c>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>259</v>
+      </c>
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>260</v>
+      </c>
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>261</v>
+      </c>
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>262</v>
+      </c>
+      <c r="B28" s="4"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>265</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B34" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6A07D0-7C3C-44CC-8F5B-0955BBFE32B4}">
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2793,170 +3059,133 @@
         <v>182</v>
       </c>
       <c r="B1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>106</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>88</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>235</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>240</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>242</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>235</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>243</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>240</v>
-      </c>
-      <c r="B12" s="4"/>
+        <v>244</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>241</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>245</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>242</v>
-      </c>
-      <c r="B14" s="4"/>
+        <v>248</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>243</v>
-      </c>
-      <c r="B15" s="4"/>
+        <v>249</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>244</v>
-      </c>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>245</v>
-      </c>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>246</v>
-      </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>248</v>
-      </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>249</v>
-      </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>251</v>
-      </c>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>254</v>
-      </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>256</v>
-      </c>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>257</v>
-      </c>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>259</v>
-      </c>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>260</v>
-      </c>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>261</v>
-      </c>
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>262</v>
-      </c>
-      <c r="B28" s="4"/>
+        <v>270</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Read 1st paper and made some notes
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC11DD66-1F67-4947-8737-1942B3E72429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBB798B-E2D6-47C1-863F-B4B28F054919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
   </bookViews>
@@ -897,7 +897,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -913,6 +913,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,8 +941,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3013,13 +3019,13 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" t="s">
         <v>71</v>
       </c>
       <c r="B32" s="4"/>
@@ -3031,7 +3037,7 @@
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="A34" t="s">
         <v>250</v>
       </c>
       <c r="B34" s="4"/>
@@ -3046,7 +3052,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3066,6 +3072,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3168,7 +3175,7 @@
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>

<commit_message>
read through extra paper
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBB798B-E2D6-47C1-863F-B4B28F054919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A52B31E-0E02-4A76-8FB1-9AD414822E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="271">
   <si>
     <t>Enhancing upper limb mobility through gamified tasks and Azure Kinect: a preliminary study in post-stroke subjects</t>
   </si>
@@ -897,7 +897,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -916,12 +916,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -935,14 +929,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3049,10 +3042,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6A07D0-7C3C-44CC-8F5B-0955BBFE32B4}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3072,125 +3065,126 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>146</v>
       </c>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>106</v>
       </c>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>88</v>
       </c>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>80</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>235</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>262</v>
+      <c r="A22" s="5" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>267</v>
+      <c r="A23" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
         <v>270</v>
       </c>
     </row>

</xml_diff>

<commit_message>
read more literature and added in introductary paragraph for the literature review which highlights the key themes identified
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A52B31E-0E02-4A76-8FB1-9AD414822E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFBEF89-3181-48FC-9392-F393B05E2CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="11928" activeTab="2" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Search" sheetId="1" r:id="rId1"/>
@@ -3044,8 +3044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6A07D0-7C3C-44CC-8F5B-0955BBFE32B4}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3107,11 +3107,13 @@
       <c r="A9" t="s">
         <v>242</v>
       </c>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>243</v>
       </c>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Yay actually started and made some progress on literature review
Done version 1 of content for theme 1: 4.5.1	Gamified Rehabilitation for Stroke
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFBEF89-3181-48FC-9392-F393B05E2CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB6A189-CA06-4314-9D15-105FF097346A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="11928" activeTab="2" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="274">
   <si>
     <t>Enhancing upper limb mobility through gamified tasks and Azure Kinect: a preliminary study in post-stroke subjects</t>
   </si>
@@ -863,6 +863,15 @@
   </si>
   <si>
     <t>Evaluating the impact of player experience in the design of a serious game for upper extremity stroke rehabilitation</t>
+  </si>
+  <si>
+    <t>An integrated low-cost system for at-home rehabilitation</t>
+  </si>
+  <si>
+    <t>Towards customizable games for stroke rehabilitation</t>
+  </si>
+  <si>
+    <t>Including gamification techniques in the design of TANGO</t>
   </si>
 </sst>
 </file>
@@ -3042,10 +3051,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6A07D0-7C3C-44CC-8F5B-0955BBFE32B4}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3075,7 +3084,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>243</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -3188,6 +3197,21 @@
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished multiplayer and haptics section
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\22754148\Downloads\Final-Year-Project-main\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB6A189-CA06-4314-9D15-105FF097346A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="11928" activeTab="2" xr2:uid="{67170054-FD0D-425F-B622-ACD1787AFD85}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Search" sheetId="1" r:id="rId1"/>
     <sheet name="Records Sought for retrieval" sheetId="2" r:id="rId2"/>
     <sheet name="Reading list" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="301">
   <si>
     <t>Enhancing upper limb mobility through gamified tasks and Azure Kinect: a preliminary study in post-stroke subjects</t>
   </si>
@@ -873,12 +872,93 @@
   <si>
     <t>Including gamification techniques in the design of TANGO</t>
   </si>
+  <si>
+    <t>In Text Reference</t>
+  </si>
+  <si>
+    <t>Ferraris et al, 2023</t>
+  </si>
+  <si>
+    <t>Strong et al, 2022</t>
+  </si>
+  <si>
+    <t>Gelineau et al, 2022</t>
+  </si>
+  <si>
+    <t>Pinto et al, 2018</t>
+  </si>
+  <si>
+    <t>Choi et al, 2018</t>
+  </si>
+  <si>
+    <t>Chen et al, 2022</t>
+  </si>
+  <si>
+    <t>Tamayo-Serrano et al, 2018</t>
+  </si>
+  <si>
+    <t>Koutsiana et al, 2020</t>
+  </si>
+  <si>
+    <t>Kecman, B, 2024</t>
+  </si>
+  <si>
+    <t>Leniston-Kahsai, S, 2020</t>
+  </si>
+  <si>
+    <t>Zhao et al, 2024</t>
+  </si>
+  <si>
+    <t>Hadjipanayi et al, 2024</t>
+  </si>
+  <si>
+    <t>Baur et al, 2018</t>
+  </si>
+  <si>
+    <t>Amorim et al, 2020</t>
+  </si>
+  <si>
+    <t>Pan, W., 2018</t>
+  </si>
+  <si>
+    <t>Doumas et al, 2021</t>
+  </si>
+  <si>
+    <t>Triandafilou et al, 2018</t>
+  </si>
+  <si>
+    <t>Vieira et al, 2021</t>
+  </si>
+  <si>
+    <t>Shahmoradi et al, 2021</t>
+  </si>
+  <si>
+    <t>Kempitiya et al, 2022</t>
+  </si>
+  <si>
+    <t>Ning et al, 2022</t>
+  </si>
+  <si>
+    <t>Cordeiro d'Ornellas et al, 2015</t>
+  </si>
+  <si>
+    <t>Borghese et al, 2012</t>
+  </si>
+  <si>
+    <t>Alankus et al, 2010</t>
+  </si>
+  <si>
+    <t>Toledo-Delgado et al, 2013</t>
+  </si>
+  <si>
+    <t>Referenced in text</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -905,8 +985,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -925,6 +1011,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -938,13 +1030,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1278,7 +1372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C08291-9268-4DC3-B18D-4AB90860BD3C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T50"/>
   <sheetViews>
@@ -1286,28 +1380,28 @@
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="50.5546875" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="50.5" customWidth="1"/>
+    <col min="2" max="2" width="8.625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="225.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="134.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="154.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="225.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="134.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="154.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>185</v>
       </c>
@@ -1369,7 +1463,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -1419,7 +1513,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -1472,7 +1566,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -1528,7 +1622,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -1581,7 +1675,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -1625,7 +1719,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1678,7 +1772,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -1734,7 +1828,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -1787,7 +1881,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -1843,7 +1937,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -1896,7 +1990,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -1946,7 +2040,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -1996,7 +2090,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -2040,7 +2134,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -2093,7 +2187,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -2152,7 +2246,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2202,7 +2296,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2255,7 +2349,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2308,7 +2402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2355,7 +2449,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2411,7 +2505,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -2467,7 +2561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
         <v>199</v>
       </c>
@@ -2517,7 +2611,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20">
       <c r="A24" t="s">
         <v>207</v>
       </c>
@@ -2570,7 +2664,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
         <v>216</v>
       </c>
@@ -2614,7 +2708,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20">
       <c r="A26" t="s">
         <v>224</v>
       </c>
@@ -2655,7 +2749,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20">
       <c r="A27" t="s">
         <v>232</v>
       </c>
@@ -2711,117 +2805,117 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20">
       <c r="D28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20">
       <c r="D29" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20">
       <c r="D30" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20">
       <c r="D31" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20">
       <c r="D32" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4">
       <c r="D33" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4">
       <c r="D34" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4">
       <c r="D35" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4">
       <c r="D36" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4">
       <c r="D37" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4">
       <c r="D38" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4">
       <c r="D39" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4">
       <c r="D40" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4">
       <c r="D41" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4">
       <c r="D42" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4">
       <c r="D43" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4">
       <c r="D44" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4">
       <c r="D45" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4">
       <c r="D46" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4">
       <c r="D47" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4">
       <c r="D48" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4">
       <c r="D49" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:4">
       <c r="D50" t="s">
         <v>262</v>
       </c>
@@ -2832,7 +2926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83627A4-1841-48FA-912D-B4DCB777AFD8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -2840,12 +2934,12 @@
       <selection activeCell="A28" activeCellId="7" sqref="A2 A3 A7:A12 A14:A17 A19:A21 A23:A24 A25:A27 A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="175.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="175.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>182</v>
       </c>
@@ -2853,192 +2947,192 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>146</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>129</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>106</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>88</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>80</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>235</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>240</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>241</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>242</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>243</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>244</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>245</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>246</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>248</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>249</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>251</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>254</v>
       </c>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>256</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>257</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>259</v>
       </c>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>260</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>261</v>
       </c>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>262</v>
       </c>
       <c r="B28" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>71</v>
       </c>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>265</v>
       </c>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>250</v>
       </c>
@@ -3050,171 +3144,264 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6A07D0-7C3C-44CC-8F5B-0955BBFE32B4}">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="164" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="141.875" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>182</v>
       </c>
       <c r="B1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>243</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>240</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>242</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>243</v>
-      </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
         <v>273</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Included the work of (Hadjipanayi et al, 2024) in the literature review
In the digital application to enhance motivation of the therapy
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\22754148\Downloads\Final-Year-Project-main\Project Writing Rescources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CFFC19-14CF-4BC6-847A-0D2A7FB5D088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Search" sheetId="1" r:id="rId1"/>
@@ -20,17 +21,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -957,8 +947,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1372,7 +1362,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T50"/>
   <sheetViews>
@@ -1380,28 +1370,28 @@
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.5" customWidth="1"/>
-    <col min="2" max="2" width="8.625" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="225.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="134.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="154.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="225.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="134.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="154.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>185</v>
       </c>
@@ -1463,7 +1453,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -1513,7 +1503,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -1566,7 +1556,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -1622,7 +1612,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -1675,7 +1665,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -1719,7 +1709,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1772,7 +1762,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -1828,7 +1818,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -1881,7 +1871,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -1937,7 +1927,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -1990,7 +1980,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -2040,7 +2030,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -2090,7 +2080,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -2134,7 +2124,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -2187,7 +2177,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -2246,7 +2236,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2296,7 +2286,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2349,7 +2339,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2402,7 +2392,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2449,7 +2439,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2505,7 +2495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -2561,7 +2551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>199</v>
       </c>
@@ -2611,7 +2601,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>207</v>
       </c>
@@ -2664,7 +2654,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>216</v>
       </c>
@@ -2708,7 +2698,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>224</v>
       </c>
@@ -2749,7 +2739,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>232</v>
       </c>
@@ -2805,117 +2795,117 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="36" spans="4:4">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="38" spans="4:4">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="4:4">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="4:4">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="41" spans="4:4">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="42" spans="4:4">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="43" spans="4:4">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="4:4">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="45" spans="4:4">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="4:4">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="4:4">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="4:4">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>262</v>
       </c>
@@ -2926,7 +2916,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -2934,12 +2924,12 @@
       <selection activeCell="A28" activeCellId="7" sqref="A2 A3 A7:A12 A14:A17 A19:A21 A23:A24 A25:A27 A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="175.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="175.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>182</v>
       </c>
@@ -2947,192 +2937,192 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>146</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>129</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>114</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>106</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>88</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>80</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>235</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>240</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>241</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>242</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>243</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>244</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>245</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>246</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>248</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>249</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>251</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>254</v>
       </c>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>256</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>257</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>259</v>
       </c>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>260</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>261</v>
       </c>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>262</v>
       </c>
       <c r="B28" s="4"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>265</v>
       </c>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>250</v>
       </c>
@@ -3144,21 +3134,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="141.875" customWidth="1"/>
+    <col min="1" max="1" width="141.88671875" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>182</v>
       </c>
@@ -3172,7 +3162,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3182,7 +3172,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -3192,7 +3182,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -3202,7 +3192,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -3212,7 +3202,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3222,7 +3212,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>235</v>
       </c>
@@ -3232,7 +3222,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>240</v>
       </c>
@@ -3242,7 +3232,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -3252,7 +3242,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>245</v>
       </c>
@@ -3261,7 +3251,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -3270,7 +3260,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -3279,15 +3269,17 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>251</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="C13" s="7"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>256</v>
       </c>
@@ -3295,7 +3287,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>257</v>
       </c>
@@ -3303,7 +3295,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>259</v>
       </c>
@@ -3312,7 +3304,7 @@
       </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>260</v>
       </c>
@@ -3321,7 +3313,7 @@
       </c>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>261</v>
       </c>
@@ -3330,7 +3322,7 @@
       </c>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>262</v>
       </c>
@@ -3339,7 +3331,7 @@
       </c>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>267</v>
       </c>
@@ -3347,15 +3339,16 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>268</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>269</v>
       </c>
@@ -3365,7 +3358,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>270</v>
       </c>
@@ -3374,7 +3367,7 @@
       </c>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>271</v>
       </c>
@@ -3383,7 +3376,7 @@
       </c>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>272</v>
       </c>
@@ -3392,7 +3385,7 @@
       </c>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>273</v>
       </c>

</xml_diff>

<commit_message>
All screened literature has been referenced
Just need to finish the digital application to enhance upper limb movement

in particular looking at the movements identified by Improving the Motivation and Participation of Elderly Patients in Rehabilitation Program Through Social Games
</commit_message>
<xml_diff>
--- a/Project Writing Rescources/Prisma retrived and screened literature.xlsx
+++ b/Project Writing Rescources/Prisma retrived and screened literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Project Writing Rescources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CFFC19-14CF-4BC6-847A-0D2A7FB5D088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E863A67F-B18C-4926-8985-5EACB4FE75E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3138,7 +3138,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3286,6 +3286,8 @@
       <c r="B14" s="6" t="s">
         <v>287</v>
       </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -3294,6 +3296,8 @@
       <c r="B15" s="6" t="s">
         <v>288</v>
       </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -3338,6 +3342,7 @@
       <c r="B20" s="6" t="s">
         <v>293</v>
       </c>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -3392,6 +3397,7 @@
       <c r="B26" s="6" t="s">
         <v>299</v>
       </c>
+      <c r="D26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>